<commit_message>
ppt modifications and RL first version
</commit_message>
<xml_diff>
--- a/resultados_execuções.xlsx
+++ b/resultados_execuções.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nokia-my.sharepoint.com/personal/lirielly_vitorugo_ext_nokia_com/Documents/TAIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{D8C93F39-37D8-4502-8549-AEA9329B5266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{408F8DE6-4FAE-41BC-8845-0F1252D82CC2}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{D8C93F39-37D8-4502-8549-AEA9329B5266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C785307B-B279-45F9-81F1-DF66A17E3D81}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B526188B-A150-4160-8888-5D860A14F4A6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>VGG1</t>
   </si>
@@ -230,6 +230,21 @@
   </si>
   <si>
     <t>EfficientNet B7</t>
+  </si>
+  <si>
+    <t>Cats</t>
+  </si>
+  <si>
+    <t>Dogs</t>
+  </si>
+  <si>
+    <t>Butterfly</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>Observations</t>
   </si>
 </sst>
 </file>
@@ -335,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -359,6 +374,7 @@
     <xf numFmtId="10" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,7 +484,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>71.587999999999994</c:v>
@@ -572,7 +588,7 @@
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>72.459999999999994</c:v>
@@ -676,7 +692,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>72.759</c:v>
@@ -710,7 +726,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -797,7 +812,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -915,7 +930,1142 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Original observations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Observations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$12:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Cats</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dogs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Butterfly</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3253</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0F6C-4F05-915A-056F308235F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1180267752"/>
+        <c:axId val="1180268080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1180267752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1180268080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1180268080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1180267752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Observations after</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> data augmentation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Observations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$17:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Cats</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dogs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6725-4A02-B0C4-FF6B0AAD3096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1180252656"/>
+        <c:axId val="1180252984"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1180252656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1180252984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1180252984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1180252656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Observations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7039-4304-8803-6DCAC228A64A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7039-4304-8803-6DCAC228A64A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7039-4304-8803-6DCAC228A64A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$12:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Cats</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dogs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Butterfly</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3253</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6E79-4A59-A3AA-7C50C827D8BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1458,6 +2608,1529 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="brightRoom" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat">
+        <a:bevelT w="50800" h="101600" prst="angle"/>
+        <a:contourClr>
+          <a:srgbClr val="000000"/>
+        </a:contourClr>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1491,6 +4164,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20309576-6BD3-4609-8495-EC4144B9F1C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{623185B7-AC75-4B24-A333-708260E8C194}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>853440</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C328B20-3E03-4F0D-A23E-B6E4CE9E36BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1796,15 +4577,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D59A954-1E67-4E13-8038-278281DA7C2B}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D8" sqref="B2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
@@ -1825,13 +4607,13 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="9">
         <v>71.587999999999994</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="9">
         <v>72.459999999999994</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="9">
         <v>72.759</v>
       </c>
     </row>
@@ -1839,13 +4621,13 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="9">
         <v>76.111000000000004</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="9">
         <v>76.921000000000006</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="9">
         <v>75.099000000000004</v>
       </c>
     </row>
@@ -1853,13 +4635,13 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="9">
         <v>78.643000000000001</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="9">
         <v>80.381</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="9">
         <v>79.453000000000003</v>
       </c>
     </row>
@@ -1867,13 +4649,13 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="9">
         <v>80.474999999999994</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="9">
         <v>83.016000000000005</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="9">
         <v>74.605000000000004</v>
       </c>
     </row>
@@ -1881,13 +4663,13 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="9">
         <v>86.765000000000001</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="9">
         <v>87.221999999999994</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="9">
         <v>86.498999999999995</v>
       </c>
     </row>
@@ -1895,13 +4677,13 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="9">
         <v>97.611000000000004</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="9">
         <v>97.81</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="9">
         <v>97.885999999999996</v>
       </c>
     </row>
@@ -1909,14 +4691,70 @@
       <c r="A8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="9">
         <v>98.677999999999997</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="9">
         <v>98.921000000000006</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="9">
         <v>98.14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>15500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18">
+        <v>15500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>